<commit_message>
[이용섭] Add - [Table] ItemTable, BasePathTable 수정, 아이템 에셋 - 테이블 바인딩
</commit_message>
<xml_diff>
--- a/Content/TableData/BasePath_Directory.xlsx
+++ b/Content/TableData/BasePath_Directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA905B-BBA1-408D-B2E8-EF619CF4CA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B6D041-5771-42D5-A730-53E6E2E7EBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42900" yWindow="5265" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{85DBA08B-C567-4CED-9E76-84B9F3389DDE}"/>
+    <workbookView xWindow="-46590" yWindow="4980" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{85DBA08B-C567-4CED-9E76-84B9F3389DDE}"/>
   </bookViews>
   <sheets>
     <sheet name="BasePath_Directory" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,14 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BP_File_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Img_File_Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,11 +98,49 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PracticeWidget_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PracticeWidget_02</t>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Level/BaseLayerLevel</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>TableData</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>UI/Widget</t>
+  </si>
+  <si>
+    <t>UI/Widget/LoadingWidget</t>
+  </si>
+  <si>
+    <t>UI/Widget/Practice</t>
+  </si>
+  <si>
+    <t>UI/Widget/Logo</t>
+  </si>
+  <si>
+    <t>UI/Widget/Account</t>
+  </si>
+  <si>
+    <t>UI/Widget/Town/Lobby</t>
+  </si>
+  <si>
+    <t>UI/Widget/Town</t>
+  </si>
+  <si>
+    <t>UI/Widget/Market</t>
+  </si>
+  <si>
+    <t>UI/Image/Icon</t>
+  </si>
+  <si>
+    <t>3D/StaticMesh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -507,7 +537,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -515,7 +545,7 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,7 +553,7 @@
         <v>201</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -531,7 +561,7 @@
         <v>301</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +569,7 @@
         <v>401</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,7 +577,7 @@
         <v>402</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +585,7 @@
         <v>1001</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -567,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E6E866-9A48-4AD1-83DB-04C0779DF277}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -579,48 +609,140 @@
     <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>301</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>401</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>402</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>402</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>403</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>404</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>405</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>406</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>407</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>408</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>409</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1001</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5001</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -653,10 +775,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -670,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>